<commit_message>
Changes to readme file.
</commit_message>
<xml_diff>
--- a/results/master_list.xlsx
+++ b/results/master_list.xlsx
@@ -53,9 +53,6 @@
     <t>chi square contingency</t>
   </si>
   <si>
-    <t>ADI</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>FM score</t>
+  </si>
+  <si>
+    <t>ARI</t>
   </si>
 </sst>
 </file>
@@ -236,15 +236,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -258,18 +270,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -590,7 +590,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,75 +610,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="14"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="O2" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
@@ -686,33 +686,33 @@
         <v>6</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="6"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3">
         <v>113.586785639087</v>
@@ -750,16 +750,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3">
         <v>274.80380476118</v>
@@ -797,16 +797,16 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3">
         <v>426.68518949964999</v>
@@ -844,16 +844,16 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="3">
         <v>111.05534938134799</v>
@@ -891,16 +891,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="3">
         <v>318.35926491286</v>
@@ -938,16 +938,16 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="3">
         <v>472.01606922288403</v>
@@ -982,12 +982,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="F1:O1"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="B1:C1"/>
@@ -997,6 +991,12 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="E1:E3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="F1:O1"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>